<commit_message>
Support for mutliple datasets added
</commit_message>
<xml_diff>
--- a/Logistic_Regression_output/Standard_classification_report.xlsx
+++ b/Logistic_Regression_output/Standard_classification_report.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7303370786516854</v>
+        <v>0.7048620983793006</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3586587436332768</v>
+        <v>0.6905292479108636</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4810703102761173</v>
+        <v>0.6976220627550302</v>
       </c>
       <c r="E2" t="n">
-        <v>2356</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3643247791333614</v>
+        <v>0.4052462526766595</v>
       </c>
       <c r="C3" t="n">
-        <v>0.735144312393888</v>
+        <v>0.4217270194986072</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4872011251758087</v>
+        <v>0.4133224133224133</v>
       </c>
       <c r="E3" t="n">
-        <v>1178</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4841539332201472</v>
+        <v>0.6009285051067781</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4841539332201472</v>
+        <v>0.6009285051067781</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4841539332201472</v>
+        <v>0.6009285051067781</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4841539332201472</v>
+        <v>0.6009285051067781</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5473309288925234</v>
+        <v>0.5550541755279801</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5469015280135824</v>
+        <v>0.5561281337047355</v>
       </c>
       <c r="D5" t="n">
-        <v>0.484135717725963</v>
+        <v>0.5554722380387218</v>
       </c>
       <c r="E5" t="n">
-        <v>3534</v>
+        <v>5385</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.608332978812244</v>
+        <v>0.6049901498117536</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4841539332201472</v>
+        <v>0.6009285051067781</v>
       </c>
       <c r="D6" t="n">
-        <v>0.483113915242681</v>
+        <v>0.602855512944158</v>
       </c>
       <c r="E6" t="n">
-        <v>3534</v>
+        <v>5385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>